<commit_message>
keep country only, remove city or county
</commit_message>
<xml_diff>
--- a/OutputData/CCHF/CCHF_Combined_11_20.xlsx
+++ b/OutputData/CCHF/CCHF_Combined_11_20.xlsx
@@ -3540,7 +3540,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Iraq:Baghdad (2), Pakistan:Karachi (2)</t>
+          <t>Iraq (2), Pakistan (2)</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -3820,7 +3820,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Nigeria (4), Russia (3), NA (3), Iraq:Baghdad (2), Pakistan:Karachi (2), Uzbekistan (1)</t>
+          <t>Nigeria (4), Russia (3), NA (3), Iraq (2), Pakistan (2), Uzbekistan (1)</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -4660,7 +4660,7 @@
       </c>
       <c r="K46" t="inlineStr">
         <is>
-          <t>Russia (5), Russia: Volgograd region (2), Russia: Stavropol region (2), Russia: Astrahan region (2)</t>
+          <t>Russia (11)</t>
         </is>
       </c>
       <c r="L46" t="inlineStr">
@@ -4752,7 +4752,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>China: Inner Mongolia (1)</t>
+          <t>China (1)</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -4844,7 +4844,7 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>China: Inner Mongolia (3)</t>
+          <t>China (3)</t>
         </is>
       </c>
       <c r="L48" t="inlineStr">
@@ -4936,7 +4936,7 @@
       </c>
       <c r="K49" t="inlineStr">
         <is>
-          <t>China: Xinjiang (1)</t>
+          <t>China (1)</t>
         </is>
       </c>
       <c r="L49" t="inlineStr">
@@ -5124,7 +5124,7 @@
       </c>
       <c r="K51" t="inlineStr">
         <is>
-          <t>Russia: Astrakhan Region (1)</t>
+          <t>Russia (1)</t>
         </is>
       </c>
       <c r="L51" t="inlineStr">
@@ -5216,7 +5216,7 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Turkey: Elicek Village/Corum (1)</t>
+          <t>Turkey (1)</t>
         </is>
       </c>
       <c r="L52" t="inlineStr">
@@ -5768,7 +5768,7 @@
       </c>
       <c r="K58" t="inlineStr">
         <is>
-          <t>NA (1), Nigeria: Sokoto (1)</t>
+          <t>NA (1), Nigeria (1)</t>
         </is>
       </c>
       <c r="L58" t="inlineStr">
@@ -6884,7 +6884,7 @@
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>Russia: Astrahan region (2), Russia: Stavropol (1), Russia: Uzbekistan (1)</t>
+          <t>Russia (4)</t>
         </is>
       </c>
       <c r="L70" t="inlineStr">
@@ -6976,7 +6976,7 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Russia: Astrahan region (1)</t>
+          <t>Russia (1)</t>
         </is>
       </c>
       <c r="L71" t="inlineStr">
@@ -7344,7 +7344,7 @@
       </c>
       <c r="K75" t="inlineStr">
         <is>
-          <t>China: Xinjiang, Bachu (2)</t>
+          <t>China (2)</t>
         </is>
       </c>
       <c r="L75" t="inlineStr">
@@ -7436,7 +7436,7 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>Nigeria: Sokoto (2)</t>
+          <t>Nigeria (2)</t>
         </is>
       </c>
       <c r="L76" t="inlineStr">
@@ -7528,7 +7528,7 @@
       </c>
       <c r="K77" t="inlineStr">
         <is>
-          <t>Pakistan: Matin (1)</t>
+          <t>Pakistan (1)</t>
         </is>
       </c>
       <c r="L77" t="inlineStr">
@@ -9582,7 +9582,7 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Russia: Volgograd Region (4), Russia: Rostov region (2), Russia: Volgograd region (1), Russia: Stavropol region (1), Russia: Rostov Region (1), Russia: Stavropole Region (1)</t>
+          <t>Russia (10)</t>
         </is>
       </c>
       <c r="L99" t="inlineStr">
@@ -9776,7 +9776,7 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Kazakhstan: Kyzylorda (3), Kazakhstan: Shyiely (2)</t>
+          <t>Kazakhstan (5)</t>
         </is>
       </c>
       <c r="L101" t="inlineStr">
@@ -9874,7 +9874,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Kazakhstan: Turkestan region (8), Kazakhstan: Shymkent (2), Kazakhstan (1)</t>
+          <t>Kazakhstan (11)</t>
         </is>
       </c>
       <c r="L102" t="inlineStr">
@@ -9972,7 +9972,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Ghana: Navrongo (3)</t>
+          <t>Ghana (3)</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -10270,7 +10270,7 @@
       </c>
       <c r="K106" t="inlineStr">
         <is>
-          <t>Turkey: Kirklareli (9)</t>
+          <t>Turkey (9)</t>
         </is>
       </c>
       <c r="L106" t="inlineStr">
@@ -10678,7 +10678,7 @@
       </c>
       <c r="K110" t="inlineStr">
         <is>
-          <t>Sudan: Al-Fulah City, Western Kordufan Province (6), Sudan: Dunkop Village, Abyei District, Western Kordufan Province (3)</t>
+          <t>Sudan (9)</t>
         </is>
       </c>
       <c r="L110" t="inlineStr">
@@ -10780,7 +10780,7 @@
       </c>
       <c r="K111" t="inlineStr">
         <is>
-          <t>Sudan: Al-Fulah City, Western Kordufan Province (2)</t>
+          <t>Sudan (2)</t>
         </is>
       </c>
       <c r="L111" t="inlineStr">
@@ -11772,7 +11772,7 @@
       </c>
       <c r="K121" t="inlineStr">
         <is>
-          <t>Ghana: Navrongo (3)</t>
+          <t>Ghana (3)</t>
         </is>
       </c>
       <c r="L121" t="inlineStr">
@@ -11972,7 +11972,7 @@
       </c>
       <c r="K123" t="inlineStr">
         <is>
-          <t>Sudan: Darfur (3)</t>
+          <t>Sudan (3)</t>
         </is>
       </c>
       <c r="L123" t="inlineStr">
@@ -12270,7 +12270,7 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Kazakhstan: Zhalagash (3)</t>
+          <t>Kazakhstan (3)</t>
         </is>
       </c>
       <c r="L126" t="inlineStr">
@@ -12372,7 +12372,7 @@
       </c>
       <c r="K127" t="inlineStr">
         <is>
-          <t>Turkey: Amasya (4)</t>
+          <t>Turkey (4)</t>
         </is>
       </c>
       <c r="L127" t="inlineStr">
@@ -12870,7 +12870,7 @@
       </c>
       <c r="K132" t="inlineStr">
         <is>
-          <t>Kosovo: Malisheve (21), Kosovo: Prishtine (10), Kosovo: Kline (8), Kosovo: Gjilan (1)</t>
+          <t>Kosovo (40)</t>
         </is>
       </c>
       <c r="L132" t="inlineStr">
@@ -13176,7 +13176,7 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>United Arab Emirates: Al Ain (15)</t>
+          <t>United Arab Emirates (15)</t>
         </is>
       </c>
       <c r="L135" t="inlineStr">
@@ -15058,7 +15058,7 @@
       </c>
       <c r="K154" t="inlineStr">
         <is>
-          <t>Russia: Kalmykia (6)</t>
+          <t>Russia (6)</t>
         </is>
       </c>
       <c r="L154" t="inlineStr">
@@ -15156,7 +15156,7 @@
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>Kazakhstan: Maktaaral district (8), Kazakhstan: Sairam district (7), Kazakhstan: South Kazakhstan oblast (3)</t>
+          <t>Kazakhstan (18)</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
@@ -15258,7 +15258,7 @@
       </c>
       <c r="K156" t="inlineStr">
         <is>
-          <t>South Africa (9), Greece (6), Senegal (6), Republic of the Congo (3), Turkey (3), Oman (3), Russia (3), Russia: Astrakhan (3), China (3), Mauritania (3)</t>
+          <t>South Africa (9), Greece (6), Russia (6), Senegal (6), Republic of the Congo (3), Turkey (3), Oman (3), China (3), Mauritania (3)</t>
         </is>
       </c>
       <c r="L156" t="inlineStr">
@@ -15870,7 +15870,7 @@
       </c>
       <c r="K162" t="inlineStr">
         <is>
-          <t>Yugoslavia: Republic of Kosovo (1)</t>
+          <t>Yugoslavia (1)</t>
         </is>
       </c>
       <c r="L162" t="inlineStr">
@@ -19874,7 +19874,7 @@
       </c>
       <c r="K202" t="inlineStr">
         <is>
-          <t>Algeria: Aflou (2)</t>
+          <t>Algeria (2)</t>
         </is>
       </c>
       <c r="L202" t="inlineStr">
@@ -20176,7 +20176,7 @@
       </c>
       <c r="K205" t="inlineStr">
         <is>
-          <t>Russia: Astrakhan (12)</t>
+          <t>Russia (12)</t>
         </is>
       </c>
       <c r="L205" t="inlineStr">
@@ -20376,7 +20376,7 @@
       </c>
       <c r="K207" t="inlineStr">
         <is>
-          <t>Tajikistan (8), Russia: Volgograd region (7), Russia (7), Russia: Stavropol region (6), Russia: Astrahan region (6), Russia: Rostov region (5), Kazakhstan (5), Russia: Volgograd Region (4), Russia: Uzbekistan (2), Russia: Tadjikistan (2), Turkmenistan (1), Uzbekistan (1), Russia: Rostov Region (1), Russia: Stavropole Region (1), Russia: Stavropol (1), Bulgaria (1)</t>
+          <t>Russia (42), Tajikistan (8), Kazakhstan (5), Turkmenistan (1), Uzbekistan (1), Bulgaria (1)</t>
         </is>
       </c>
       <c r="L207" t="inlineStr">
@@ -20776,7 +20776,7 @@
       </c>
       <c r="K211" t="inlineStr">
         <is>
-          <t>Tajikistan (8), NA (8), Russia: Rostov region (6), Kazakhstan (5), Russia: Volgograd region (4), Russia: Stavropol region (4), Russia: Astrahan region (4), Russia (2), Turkmenistan (1), Uzbekistan (1), Russia: Tadjikistan (1), Russia: Stavropol (1), Russia: Uzbekistan (1), Bulgaria (1)</t>
+          <t>Russia (23), Tajikistan (8), NA (8), Kazakhstan (5), Turkmenistan (1), Uzbekistan (1), Bulgaria (1)</t>
         </is>
       </c>
       <c r="L211" t="inlineStr">
@@ -20878,7 +20878,7 @@
       </c>
       <c r="K212" t="inlineStr">
         <is>
-          <t>Russia: Rostov (9), Russia: Stavropol (9), Russia: Astrakhan (6), Turkmenistan (6), Uganda (3), Kazakhstan (3), Nigeria (3), Uzbekistan (3), Tajikistan (3)</t>
+          <t>Russia (24), Turkmenistan (6), Uganda (3), Kazakhstan (3), Nigeria (3), Uzbekistan (3), Tajikistan (3)</t>
         </is>
       </c>
       <c r="L212" t="inlineStr">
@@ -22070,7 +22070,7 @@
       </c>
       <c r="K224" t="inlineStr">
         <is>
-          <t>Russia: Rostov region (2)</t>
+          <t>Russia (2)</t>
         </is>
       </c>
       <c r="L224" t="inlineStr">
@@ -22172,7 +22172,7 @@
       </c>
       <c r="K225" t="inlineStr">
         <is>
-          <t>Russia (8), Tajikistan (2), Russia: Astrakhan Region (1), Bulgaria (1), Turkmenistan (1), Uzbekistan (1)</t>
+          <t>Russia (9), Tajikistan (2), Bulgaria (1), Turkmenistan (1), Uzbekistan (1)</t>
         </is>
       </c>
       <c r="L225" t="inlineStr">
@@ -22274,7 +22274,7 @@
       </c>
       <c r="K226" t="inlineStr">
         <is>
-          <t>Tajikistan (1), Russia: Astrakhan region (1)</t>
+          <t>Tajikistan (1), Russia (1)</t>
         </is>
       </c>
       <c r="L226" t="inlineStr">
@@ -23070,7 +23070,7 @@
       </c>
       <c r="K234" t="inlineStr">
         <is>
-          <t>China:Xinjiang province (7)</t>
+          <t>China (7)</t>
         </is>
       </c>
       <c r="L234" t="inlineStr">
@@ -23568,7 +23568,7 @@
       </c>
       <c r="K239" t="inlineStr">
         <is>
-          <t>Russia: Astrakhan region, Narimanovsky district (3)</t>
+          <t>Russia (3)</t>
         </is>
       </c>
       <c r="L239" t="inlineStr">
@@ -23768,7 +23768,7 @@
       </c>
       <c r="K241" t="inlineStr">
         <is>
-          <t>Uganda: Kikuube district (2)</t>
+          <t>Uganda (2)</t>
         </is>
       </c>
       <c r="L241" t="inlineStr">
@@ -23968,7 +23968,7 @@
       </c>
       <c r="K243" t="inlineStr">
         <is>
-          <t>Kenya: Baringo County (7), Kenya: Kajiado County (1)</t>
+          <t>Kenya (8)</t>
         </is>
       </c>
       <c r="L243" t="inlineStr">
@@ -24964,7 +24964,7 @@
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t>Turkey: Kastomonu (2)</t>
+          <t>Turkey (2)</t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
@@ -25674,7 +25674,7 @@
       </c>
       <c r="K260" t="inlineStr">
         <is>
-          <t>Greece: Rodopi (1), Greece: Rodopi prefecture (1)</t>
+          <t>Greece (2)</t>
         </is>
       </c>
       <c r="L260" t="inlineStr">
@@ -26078,7 +26078,7 @@
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t>Greece:North, Kastoria (1)</t>
+          <t>Greece (1)</t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
@@ -26572,7 +26572,7 @@
       </c>
       <c r="K269" t="inlineStr">
         <is>
-          <t>Russia: Volgograd region (3), Russia: Stavropol region (2), Russia: Astrahan region (1)</t>
+          <t>Russia (6)</t>
         </is>
       </c>
       <c r="L269" t="inlineStr">
@@ -26772,7 +26772,7 @@
       </c>
       <c r="K271" t="inlineStr">
         <is>
-          <t>Tajikistan: Rudaki region (3)</t>
+          <t>Tajikistan (3)</t>
         </is>
       </c>
       <c r="L271" t="inlineStr">
@@ -26870,7 +26870,7 @@
       </c>
       <c r="K272" t="inlineStr">
         <is>
-          <t>Tajikistan: Tursunzade region (9)</t>
+          <t>Tajikistan (9)</t>
         </is>
       </c>
       <c r="L272" t="inlineStr">
@@ -27768,7 +27768,7 @@
       </c>
       <c r="K281" t="inlineStr">
         <is>
-          <t>India: Gujarat State (66), India: Rajasthan State (30), India: Gujarat State, Bhavnagar (15), India: Amreli District, Gujarat State (9), India: Gujarat State,Amreli (6), India: Rajkot District, Gujarat State (6), India: Vadodara District, Gujarat State (6), India: Bhuj District, Gujarat State (6), India: Kutch District, Gujarat State (6), India: Gujarat State,Surendra Nagar (3), India: Rajasthan State,Sirohi (3), India: Gujarat State,Bhavnagar (3), India: Jodhpur District, Rajasthan State (3), India: Ahmadabad District, Gujarat State (3)</t>
+          <t>India (165)</t>
         </is>
       </c>
       <c r="L281" t="inlineStr">
@@ -27968,7 +27968,7 @@
       </c>
       <c r="K283" t="inlineStr">
         <is>
-          <t>China: Xinjiang Uygur Autonomous Region (15), China: Xinjiang, Bachu (2)</t>
+          <t>China (17)</t>
         </is>
       </c>
       <c r="L283" t="inlineStr">
@@ -28266,7 +28266,7 @@
       </c>
       <c r="K286" t="inlineStr">
         <is>
-          <t>Nigeria: Sokoto (2), Pakistan: Matin (1)</t>
+          <t>Nigeria (2), Pakistan (1)</t>
         </is>
       </c>
       <c r="L286" t="inlineStr">
@@ -28564,7 +28564,7 @@
       </c>
       <c r="K289" t="inlineStr">
         <is>
-          <t>Russia (1), Russia: Volgograd (1), Tajikistan (1)</t>
+          <t>Russia (2), Tajikistan (1)</t>
         </is>
       </c>
       <c r="L289" t="inlineStr">
@@ -29062,7 +29062,7 @@
       </c>
       <c r="K294" t="inlineStr">
         <is>
-          <t>Turkey: Antakya (1), Turkey: Hassa (1), Syria: Kafr Takharim (1), Syria: Qalat Samaan (1)</t>
+          <t>Turkey (2), Syria (2)</t>
         </is>
       </c>
       <c r="L294" t="inlineStr">
@@ -29356,7 +29356,7 @@
       </c>
       <c r="K297" t="inlineStr">
         <is>
-          <t>USA: MD (5)</t>
+          <t>USA (5)</t>
         </is>
       </c>
       <c r="L297" t="inlineStr">
@@ -29454,7 +29454,7 @@
       </c>
       <c r="K298" t="inlineStr">
         <is>
-          <t>NA (2), China (1), China: XinJiang (1)</t>
+          <t>China (2), NA (2)</t>
         </is>
       </c>
       <c r="L298" t="inlineStr">
@@ -29552,7 +29552,7 @@
       </c>
       <c r="K299" t="inlineStr">
         <is>
-          <t>China (1), China: XinJiang (1)</t>
+          <t>China (2)</t>
         </is>
       </c>
       <c r="L299" t="inlineStr">
@@ -30246,7 +30246,7 @@
       </c>
       <c r="K306" t="inlineStr">
         <is>
-          <t>Russia: Astrakhan region (3)</t>
+          <t>Russia (3)</t>
         </is>
       </c>
       <c r="L306" t="inlineStr">
@@ -30344,7 +30344,7 @@
       </c>
       <c r="K307" t="inlineStr">
         <is>
-          <t>Uganda: Kampala (3)</t>
+          <t>Uganda (3)</t>
         </is>
       </c>
       <c r="L307" t="inlineStr">
@@ -30442,7 +30442,7 @@
       </c>
       <c r="K308" t="inlineStr">
         <is>
-          <t>Turkey: Aktas (2), Turkey: Cevrecik (1)</t>
+          <t>Turkey (3)</t>
         </is>
       </c>
       <c r="L308" t="inlineStr">
@@ -30540,7 +30540,7 @@
       </c>
       <c r="K309" t="inlineStr">
         <is>
-          <t>India (23), India: Kutch (1)</t>
+          <t>India (24)</t>
         </is>
       </c>
       <c r="L309" t="inlineStr">
@@ -30740,7 +30740,7 @@
       </c>
       <c r="K311" t="inlineStr">
         <is>
-          <t>India: Gujarat State, Bhavnagar (11), India: Gujarat State, Amreli (5), India: Rajasthan State, Sirohi (2), India: Gujarat State, Surendra Nagar (1), India: Gujarat State, Rajkot (1), India: Gujarat State, Anand (1)</t>
+          <t>India (21)</t>
         </is>
       </c>
       <c r="L311" t="inlineStr">
@@ -30838,7 +30838,7 @@
       </c>
       <c r="K312" t="inlineStr">
         <is>
-          <t>Russia: Stavropol (14)</t>
+          <t>Russia (14)</t>
         </is>
       </c>
       <c r="L312" t="inlineStr">
@@ -31038,7 +31038,7 @@
       </c>
       <c r="K314" t="inlineStr">
         <is>
-          <t>Saudi Arabia: Al-Khurma (3)</t>
+          <t>Saudi Arabia (3)</t>
         </is>
       </c>
       <c r="L314" t="inlineStr">
@@ -31136,7 +31136,7 @@
       </c>
       <c r="K315" t="inlineStr">
         <is>
-          <t>Turkey: Istanbul (11)</t>
+          <t>Turkey (11)</t>
         </is>
       </c>
       <c r="L315" t="inlineStr">
@@ -31728,7 +31728,7 @@
       </c>
       <c r="K321" t="inlineStr">
         <is>
-          <t>Mali: Daral (3)</t>
+          <t>Mali (3)</t>
         </is>
       </c>
       <c r="L321" t="inlineStr">

</xml_diff>